<commit_message>
Fix: mathstat lab1 report
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
+++ b/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\MathStat\tasks\task5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Doc\ITMO-graevsky\2COURSE\2SEM\MathStat\tasks\task5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4849DE-964C-445D-87E9-72F6257DDCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F316D8-7FF4-4DC6-904B-668C6C01DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{32CC6188-2725-4CF5-B55F-61B73774C570}"/>
+    <workbookView xWindow="28440" yWindow="0" windowWidth="17265" windowHeight="15780" xr2:uid="{32CC6188-2725-4CF5-B55F-61B73774C570}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -292,7 +292,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -354,7 +354,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -518,7 +518,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="302575007"/>
@@ -580,7 +580,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="302565407"/>
@@ -628,7 +628,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -642,7 +642,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -708,7 +708,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -960,7 +960,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="307439119"/>
@@ -1022,7 +1022,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="307417039"/>
@@ -1064,7 +1064,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1101,7 +1101,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2302,9 +2302,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2342,7 +2342,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2448,7 +2448,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2600,26 +2600,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DCC99B-EDBB-481C-8A26-B6D3FDF71907}">
   <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" customWidth="1"/>
+    <col min="26" max="26" width="21.28515625" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" customWidth="1"/>
-    <col min="30" max="32" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>-98.3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>SUM(B2:G2)</f>
         <v>120</v>
@@ -2822,7 +2822,7 @@
         <v>-3017.7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
@@ -2835,7 +2835,7 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
         <v>44</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -2987,7 +2987,7 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -3000,7 +3000,7 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -3044,7 +3044,7 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C22">
         <f>-SUM(B2:G2)</f>
         <v>-120</v>
@@ -3085,7 +3085,7 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
@@ -3098,7 +3098,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -3142,7 +3142,7 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>3.5587188612099648E-2</v>
       </c>
@@ -3161,7 +3161,7 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -3180,7 +3180,7 @@
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -3201,7 +3201,7 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -3225,7 +3225,7 @@
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q30" s="2"/>
       <c r="R30" s="2" t="s">
         <v>46</v>
@@ -3248,7 +3248,7 @@
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q31" s="2"/>
       <c r="R31" s="2" t="s">
         <v>45</v>
@@ -3269,7 +3269,7 @@
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Q32" s="2"/>
       <c r="R32" s="2">
         <v>2.78</v>
@@ -3290,7 +3290,7 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
-    <row r="33" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -3316,7 +3316,7 @@
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
     </row>
-    <row r="34" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -3339,7 +3339,7 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -3358,7 +3358,7 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
     </row>
-    <row r="36" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
@@ -3379,7 +3379,7 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
-    <row r="37" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
@@ -3413,7 +3413,7 @@
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
     </row>
-    <row r="38" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Y38" s="2"/>
       <c r="Z38" s="2" t="s">
         <v>52</v>
@@ -3446,7 +3446,7 @@
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
     </row>
-    <row r="39" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
@@ -3459,7 +3459,7 @@
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
     </row>
-    <row r="41" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z41" s="2" t="s">
         <v>42</v>
       </c>
@@ -3467,13 +3467,13 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
     </row>
-    <row r="42" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
     </row>
-    <row r="43" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z43" s="2" t="s">
         <v>25</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
     </row>
-    <row r="44" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z44" s="2"/>
       <c r="AA44" s="2" t="s">
         <v>49</v>
@@ -3491,19 +3491,19 @@
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
     </row>
-    <row r="45" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
     </row>
-    <row r="46" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
     </row>
-    <row r="47" spans="17:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Z47" s="2" t="s">
         <v>26</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
     </row>
-    <row r="49" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="49" spans="26:32" x14ac:dyDescent="0.25">
       <c r="Z49" s="2" t="s">
         <v>51</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
     </row>
-    <row r="50" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="50" spans="26:32" x14ac:dyDescent="0.25">
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
@@ -3533,7 +3533,7 @@
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
     </row>
-    <row r="51" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="51" spans="26:32" x14ac:dyDescent="0.25">
       <c r="Z51" s="2" t="s">
         <v>37</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="52" spans="26:32" x14ac:dyDescent="0.25">
       <c r="Z52" s="2" t="s">
         <v>53</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>-42.582265717674936</v>
       </c>
     </row>
-    <row r="53" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="53" spans="26:32" x14ac:dyDescent="0.25">
       <c r="Z53" s="2" t="s">
         <v>54</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>-42.582265717674936</v>
       </c>
     </row>
-    <row r="57" spans="26:32" x14ac:dyDescent="0.3">
+    <row r="57" spans="26:32" x14ac:dyDescent="0.25">
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
     </row>

</xml_diff>

<commit_message>
CSA Lab 3 minor fix
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
+++ b/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Doc\ITMO-graevsky\2COURSE\2SEM\MathStat\tasks\task5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\MathStat\tasks\task5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F316D8-7FF4-4DC6-904B-668C6C01DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F3E8E6-6606-422D-8772-1E70C2EA7FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28440" yWindow="0" windowWidth="17265" windowHeight="15780" xr2:uid="{32CC6188-2725-4CF5-B55F-61B73774C570}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{32CC6188-2725-4CF5-B55F-61B73774C570}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Нужно</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>\ov{y}+\gamma\sigma(y)</t>
+  </si>
+  <si>
+    <t>21,044-2,78*sqrt{0,007}</t>
+  </si>
+  <si>
+    <t>&lt;a_0&lt;</t>
+  </si>
+  <si>
+    <t>21,044+2,78*sqrt{0.007}</t>
+  </si>
+  <si>
+    <t>-1,871-2,78*sqrt{3,243}</t>
+  </si>
+  <si>
+    <t>&lt;a_1&lt;</t>
+  </si>
+  <si>
+    <t>-1,871+2,78*sqrt{3,243}</t>
   </si>
 </sst>
 </file>
@@ -266,15 +284,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -292,7 +313,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -354,7 +375,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -518,7 +539,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="302575007"/>
@@ -580,7 +601,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="302565407"/>
@@ -628,7 +649,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -642,7 +663,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -708,7 +729,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -960,7 +981,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="307439119"/>
@@ -1022,7 +1043,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="307417039"/>
@@ -1064,7 +1085,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1101,7 +1122,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2302,9 +2323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2342,7 +2363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2448,7 +2469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2598,28 +2619,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DCC99B-EDBB-481C-8A26-B6D3FDF71907}">
-  <dimension ref="A1:AI57"/>
+  <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.28515625" customWidth="1"/>
+    <col min="26" max="26" width="21.33203125" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" customWidth="1"/>
+    <col min="30" max="32" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2627,7 +2648,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2662,7 +2683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2691,7 +2712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2758,7 +2779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2776,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2826,7 @@
         <v>-98.3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C11">
         <f>SUM(B2:G2)</f>
         <v>120</v>
@@ -2822,7 +2843,7 @@
         <v>-3017.7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
@@ -2835,7 +2856,7 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2880,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -2887,7 +2908,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -2934,7 +2955,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
       <c r="M18" t="s">
         <v>44</v>
       </c>
@@ -2974,7 +2995,7 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -2987,7 +3008,7 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -3000,7 +3021,7 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -3044,7 +3065,7 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
       <c r="C22">
         <f>-SUM(B2:G2)</f>
         <v>-120</v>
@@ -3085,7 +3106,7 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
@@ -3098,7 +3119,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -3114,7 +3135,7 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -3142,7 +3163,7 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>3.5587188612099648E-2</v>
       </c>
@@ -3161,7 +3182,7 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -3180,7 +3201,7 @@
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -3201,7 +3222,7 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -3225,7 +3246,7 @@
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q30" s="2"/>
       <c r="R30" s="2" t="s">
         <v>46</v>
@@ -3248,7 +3269,7 @@
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q31" s="2"/>
       <c r="R31" s="2" t="s">
         <v>45</v>
@@ -3269,7 +3290,7 @@
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
       <c r="Q32" s="2"/>
       <c r="R32" s="2">
         <v>2.78</v>
@@ -3290,7 +3311,7 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
-    <row r="33" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -3316,7 +3337,7 @@
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
     </row>
-    <row r="34" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -3339,7 +3360,7 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -3358,7 +3379,7 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
     </row>
-    <row r="36" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
@@ -3379,7 +3400,7 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
-    <row r="37" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
@@ -3413,7 +3434,7 @@
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
     </row>
-    <row r="38" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Y38" s="2"/>
       <c r="Z38" s="2" t="s">
         <v>52</v>
@@ -3446,7 +3467,7 @@
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
     </row>
-    <row r="39" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
@@ -3459,7 +3480,7 @@
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
     </row>
-    <row r="41" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z41" s="2" t="s">
         <v>42</v>
       </c>
@@ -3467,13 +3488,13 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
     </row>
-    <row r="42" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
     </row>
-    <row r="43" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z43" s="2" t="s">
         <v>25</v>
       </c>
@@ -3482,28 +3503,54 @@
       </c>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
-    </row>
-    <row r="44" spans="17:35" x14ac:dyDescent="0.25">
+      <c r="AD43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z44" s="2"/>
       <c r="AA44" s="2" t="s">
         <v>49</v>
       </c>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-    </row>
-    <row r="45" spans="17:35" x14ac:dyDescent="0.25">
+      <c r="AE44">
+        <v>20.811</v>
+      </c>
+      <c r="AG44">
+        <v>21.277000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
     </row>
-    <row r="46" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
-      <c r="AC46" s="2"/>
-    </row>
-    <row r="47" spans="17:35" x14ac:dyDescent="0.25">
+      <c r="AC46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD46" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG46" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z47" s="2" t="s">
         <v>26</v>
       </c>
@@ -3512,8 +3559,17 @@
       </c>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-    </row>
-    <row r="49" spans="26:32" x14ac:dyDescent="0.25">
+      <c r="AE47">
+        <v>-6.8769999999999998</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG47">
+        <v>3.1349999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="26:41" x14ac:dyDescent="0.3">
       <c r="Z49" s="2" t="s">
         <v>51</v>
       </c>
@@ -3524,7 +3580,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
     </row>
-    <row r="50" spans="26:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="26:41" x14ac:dyDescent="0.3">
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
@@ -3532,8 +3588,16 @@
       <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
-    </row>
-    <row r="51" spans="26:32" x14ac:dyDescent="0.25">
+      <c r="AH50" s="6"/>
+      <c r="AI50" s="6"/>
+      <c r="AJ50" s="6"/>
+      <c r="AK50" s="6"/>
+      <c r="AL50" s="6"/>
+      <c r="AM50" s="6"/>
+      <c r="AN50" s="6"/>
+      <c r="AO50" s="6"/>
+    </row>
+    <row r="51" spans="26:41" x14ac:dyDescent="0.3">
       <c r="Z51" s="2" t="s">
         <v>37</v>
       </c>
@@ -3561,8 +3625,16 @@
         <f>AF37</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="26:32" x14ac:dyDescent="0.25">
+      <c r="AH51" s="6"/>
+      <c r="AI51" s="6"/>
+      <c r="AJ51" s="6"/>
+      <c r="AK51" s="6"/>
+      <c r="AL51" s="6"/>
+      <c r="AM51" s="6"/>
+      <c r="AN51" s="6"/>
+      <c r="AO51" s="6"/>
+    </row>
+    <row r="52" spans="26:41" x14ac:dyDescent="0.3">
       <c r="Z52" s="2" t="s">
         <v>53</v>
       </c>
@@ -3590,8 +3662,16 @@
         <f t="shared" si="8"/>
         <v>-42.582265717674936</v>
       </c>
-    </row>
-    <row r="53" spans="26:32" x14ac:dyDescent="0.25">
+      <c r="AH52" s="6"/>
+      <c r="AI52" s="7"/>
+      <c r="AJ52" s="7"/>
+      <c r="AK52" s="7"/>
+      <c r="AL52" s="7"/>
+      <c r="AM52" s="7"/>
+      <c r="AN52" s="7"/>
+      <c r="AO52" s="6"/>
+    </row>
+    <row r="53" spans="26:41" x14ac:dyDescent="0.3">
       <c r="Z53" s="2" t="s">
         <v>54</v>
       </c>
@@ -3619,8 +3699,36 @@
         <f t="shared" si="9"/>
         <v>-42.582265717674936</v>
       </c>
-    </row>
-    <row r="57" spans="26:32" x14ac:dyDescent="0.25">
+      <c r="AH53" s="6"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7"/>
+      <c r="AL53" s="7"/>
+      <c r="AM53" s="7"/>
+      <c r="AN53" s="7"/>
+      <c r="AO53" s="6"/>
+    </row>
+    <row r="54" spans="26:41" x14ac:dyDescent="0.3">
+      <c r="AH54" s="6"/>
+      <c r="AI54" s="6"/>
+      <c r="AJ54" s="6"/>
+      <c r="AK54" s="6"/>
+      <c r="AL54" s="6"/>
+      <c r="AM54" s="6"/>
+      <c r="AN54" s="6"/>
+      <c r="AO54" s="6"/>
+    </row>
+    <row r="55" spans="26:41" x14ac:dyDescent="0.3">
+      <c r="AH55" s="6"/>
+      <c r="AI55" s="6"/>
+      <c r="AJ55" s="6"/>
+      <c r="AK55" s="6"/>
+      <c r="AL55" s="6"/>
+      <c r="AM55" s="6"/>
+      <c r="AN55" s="6"/>
+      <c r="AO55" s="6"/>
+    </row>
+    <row r="57" spans="26:41" x14ac:dyDescent="0.3">
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
     </row>

</xml_diff>

<commit_message>
CSA Lab 3 if cond jump
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
+++ b/2COURSE/2SEM/MathStat/tasks/task5/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\MathStat\tasks\task5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F3E8E6-6606-422D-8772-1E70C2EA7FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771B085-89F5-46B0-8BC9-6992669B3737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{32CC6188-2725-4CF5-B55F-61B73774C570}"/>
   </bookViews>
@@ -223,22 +223,22 @@
     <t>\ov{y}+\gamma\sigma(y)</t>
   </si>
   <si>
-    <t>21,044-2,78*sqrt{0,007}</t>
-  </si>
-  <si>
-    <t>&lt;a_0&lt;</t>
-  </si>
-  <si>
-    <t>21,044+2,78*sqrt{0.007}</t>
-  </si>
-  <si>
-    <t>-1,871-2,78*sqrt{3,243}</t>
-  </si>
-  <si>
-    <t>&lt;a_1&lt;</t>
-  </si>
-  <si>
-    <t>-1,871+2,78*sqrt{3,243}</t>
+    <t>21,044-2,78*sqrt{3,243}</t>
+  </si>
+  <si>
+    <t>&lt; a_0 &lt;</t>
+  </si>
+  <si>
+    <t>21,044+2,78*sqrt{3,243}</t>
+  </si>
+  <si>
+    <t>-1,871-2,78*sqrt{0,007}</t>
+  </si>
+  <si>
+    <t>&lt; a_1 &lt;</t>
+  </si>
+  <si>
+    <t>-1,871+2,78*sqrt{0,007}</t>
   </si>
 </sst>
 </file>
@@ -284,15 +284,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -800,22 +798,22 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-13.547233055143098</c:v>
+                  <c:v>7.6647607229927202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4125148279952384</c:v>
+                  <c:v>-4.2417189059098126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12.64062870699879</c:v>
+                  <c:v>-14.867358475904695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-21.997390272835091</c:v>
+                  <c:v>-24.280406841170681</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-31.354151838671385</c:v>
+                  <c:v>-34.18335591658596</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-42.582265717674936</c:v>
+                  <c:v>-46.417073439862996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,22 +886,22 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.92113578349425</c:v>
+                  <c:v>15.70914200535843</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4125148279952384</c:v>
+                  <c:v>1.4166892499193358</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12.64062870699879</c:v>
+                  <c:v>-10.413898938092885</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-21.997390272835091</c:v>
+                  <c:v>-19.714373704499501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-31.354151838671385</c:v>
+                  <c:v>-28.52494776075681</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-42.582265717674936</c:v>
+                  <c:v>-38.747457995486876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DCC99B-EDBB-481C-8A26-B6D3FDF71907}">
-  <dimension ref="A1:AO57"/>
+  <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W47" sqref="W47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y51" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3140,11 +3138,11 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" cm="1">
-        <f t="array" ref="C25:D26">C10:D11*D17</f>
-        <v>1.7793594306049823E-3</v>
+        <f t="array" ref="C25:D26">C21:D22*D17</f>
+        <v>0.87841043890865966</v>
       </c>
       <c r="D25" s="1">
-        <v>3.5587188612099648E-2</v>
+        <v>-3.5587188612099648E-2</v>
       </c>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2" t="s">
@@ -3165,10 +3163,10 @@
     </row>
     <row r="26" spans="2:35" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
-        <v>3.5587188612099648E-2</v>
+        <v>-3.5587188612099648E-2</v>
       </c>
       <c r="D26" s="1">
-        <v>0.87841043890865966</v>
+        <v>1.7793594306049823E-3</v>
       </c>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
@@ -3324,10 +3322,10 @@
       </c>
       <c r="AA33" s="3" cm="1">
         <f t="array" ref="AA33:AB34">AA29*C25:D26</f>
-        <v>6.5689971420490349E-3</v>
+        <v>3.2428949224582073</v>
       </c>
       <c r="AB33" s="3">
-        <v>0.1313799428409807</v>
+        <v>-0.1313799428409807</v>
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
@@ -3347,10 +3345,10 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="3">
-        <v>0.1313799428409807</v>
+        <v>-0.1313799428409807</v>
       </c>
       <c r="AB34" s="3">
-        <v>3.2428949224582073</v>
+        <v>6.5689971420490349E-3</v>
       </c>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
@@ -3441,27 +3439,27 @@
       </c>
       <c r="AA38" s="3">
         <f>$AA$33+2*$AB$33*AA37+$AB$34*AA37*AA37</f>
-        <v>82.392741487007044</v>
+        <v>2.0933204225996263</v>
       </c>
       <c r="AB38" s="3">
         <f>$AA$33+2*$AB$33*AB37+$AB$34*AB37*AB37</f>
-        <v>470.13655645930743</v>
+        <v>1.0357118827297316</v>
       </c>
       <c r="AC38" s="3">
         <f t="shared" ref="AC38:AF38" si="6">$AA$33+2*$AB$33*AC37+$AB$34*AC37*AC37</f>
-        <v>1055.4342018158763</v>
+        <v>0.64157205420678887</v>
       </c>
       <c r="AD38" s="3">
         <f t="shared" si="6"/>
-        <v>1721.5414603482191</v>
+        <v>0.67441703991703461</v>
       </c>
       <c r="AE38" s="3">
         <f t="shared" si="6"/>
-        <v>2549.7934650034717</v>
+        <v>1.035711882729732</v>
       </c>
       <c r="AF38" s="3">
         <f t="shared" si="6"/>
-        <v>3757.7269354720165</v>
+        <v>1.9028195054802035</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
@@ -3521,10 +3519,13 @@
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
       <c r="AE44">
-        <v>20.811</v>
+        <v>16.038</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>56</v>
       </c>
       <c r="AG44">
-        <v>21.277000000000001</v>
+        <v>26.05</v>
       </c>
     </row>
     <row r="45" spans="17:35" x14ac:dyDescent="0.3">
@@ -3537,18 +3538,7 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
-      <c r="AC46" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD46" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG46" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC46" s="2"/>
     </row>
     <row r="47" spans="17:35" x14ac:dyDescent="0.3">
       <c r="Z47" s="2" t="s">
@@ -3559,17 +3549,28 @@
       </c>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-      <c r="AE47">
-        <v>-6.8769999999999998</v>
+      <c r="AD47" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="AF47" t="s">
         <v>59</v>
       </c>
-      <c r="AG47">
-        <v>3.1349999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="26:41" x14ac:dyDescent="0.3">
+      <c r="AG47" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="17:35" x14ac:dyDescent="0.3">
+      <c r="AE48">
+        <v>-2.1040000000000001</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG48">
+        <v>-1.6379999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="26:32" x14ac:dyDescent="0.3">
       <c r="Z49" s="2" t="s">
         <v>51</v>
       </c>
@@ -3580,7 +3581,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
     </row>
-    <row r="50" spans="26:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="26:32" x14ac:dyDescent="0.3">
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
@@ -3588,16 +3589,8 @@
       <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
-      <c r="AH50" s="6"/>
-      <c r="AI50" s="6"/>
-      <c r="AJ50" s="6"/>
-      <c r="AK50" s="6"/>
-      <c r="AL50" s="6"/>
-      <c r="AM50" s="6"/>
-      <c r="AN50" s="6"/>
-      <c r="AO50" s="6"/>
-    </row>
-    <row r="51" spans="26:41" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="26:32" x14ac:dyDescent="0.3">
       <c r="Z51" s="2" t="s">
         <v>37</v>
       </c>
@@ -3625,110 +3618,66 @@
         <f>AF37</f>
         <v>34</v>
       </c>
-      <c r="AH51" s="6"/>
-      <c r="AI51" s="6"/>
-      <c r="AJ51" s="6"/>
-      <c r="AK51" s="6"/>
-      <c r="AL51" s="6"/>
-      <c r="AM51" s="6"/>
-      <c r="AN51" s="6"/>
-      <c r="AO51" s="6"/>
-    </row>
-    <row r="52" spans="26:41" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="26:32" x14ac:dyDescent="0.3">
       <c r="Z52" s="2" t="s">
         <v>53</v>
       </c>
       <c r="AA52" s="3">
-        <f>AA18-R32*SQRT(AA38)</f>
-        <v>-13.547233055143098</v>
+        <f>AA18-$R$32*SQRT(AA38)</f>
+        <v>7.6647607229927202</v>
       </c>
       <c r="AB52" s="3">
-        <f t="shared" ref="AB52:AF52" si="8">AB18-S32*SQRT(AB38)</f>
-        <v>-1.4125148279952384</v>
+        <f t="shared" ref="AB52:AF52" si="8">AB18-$R$32*SQRT(AB38)</f>
+        <v>-4.2417189059098126</v>
       </c>
       <c r="AC52" s="3">
         <f t="shared" si="8"/>
-        <v>-12.64062870699879</v>
+        <v>-14.867358475904695</v>
       </c>
       <c r="AD52" s="3">
         <f t="shared" si="8"/>
-        <v>-21.997390272835091</v>
+        <v>-24.280406841170681</v>
       </c>
       <c r="AE52" s="3">
         <f t="shared" si="8"/>
-        <v>-31.354151838671385</v>
+        <v>-34.18335591658596</v>
       </c>
       <c r="AF52" s="3">
         <f t="shared" si="8"/>
-        <v>-42.582265717674936</v>
-      </c>
-      <c r="AH52" s="6"/>
-      <c r="AI52" s="7"/>
-      <c r="AJ52" s="7"/>
-      <c r="AK52" s="7"/>
-      <c r="AL52" s="7"/>
-      <c r="AM52" s="7"/>
-      <c r="AN52" s="7"/>
-      <c r="AO52" s="6"/>
-    </row>
-    <row r="53" spans="26:41" x14ac:dyDescent="0.3">
+        <v>-46.417073439862996</v>
+      </c>
+    </row>
+    <row r="53" spans="26:32" x14ac:dyDescent="0.3">
       <c r="Z53" s="2" t="s">
         <v>54</v>
       </c>
       <c r="AA53" s="3">
-        <f>AA18+R32*SQRT(AA38)</f>
-        <v>36.92113578349425</v>
+        <f>AA18+$R$32*SQRT(AA38)</f>
+        <v>15.70914200535843</v>
       </c>
       <c r="AB53" s="3">
-        <f t="shared" ref="AB53:AF53" si="9">AB18+S32*SQRT(AB38)</f>
-        <v>-1.4125148279952384</v>
+        <f t="shared" ref="AB53:AF53" si="9">AB18+$R$32*SQRT(AB38)</f>
+        <v>1.4166892499193358</v>
       </c>
       <c r="AC53" s="3">
         <f t="shared" si="9"/>
-        <v>-12.64062870699879</v>
+        <v>-10.413898938092885</v>
       </c>
       <c r="AD53" s="3">
         <f t="shared" si="9"/>
-        <v>-21.997390272835091</v>
+        <v>-19.714373704499501</v>
       </c>
       <c r="AE53" s="3">
         <f t="shared" si="9"/>
-        <v>-31.354151838671385</v>
+        <v>-28.52494776075681</v>
       </c>
       <c r="AF53" s="3">
         <f t="shared" si="9"/>
-        <v>-42.582265717674936</v>
-      </c>
-      <c r="AH53" s="6"/>
-      <c r="AI53" s="7"/>
-      <c r="AJ53" s="7"/>
-      <c r="AK53" s="7"/>
-      <c r="AL53" s="7"/>
-      <c r="AM53" s="7"/>
-      <c r="AN53" s="7"/>
-      <c r="AO53" s="6"/>
-    </row>
-    <row r="54" spans="26:41" x14ac:dyDescent="0.3">
-      <c r="AH54" s="6"/>
-      <c r="AI54" s="6"/>
-      <c r="AJ54" s="6"/>
-      <c r="AK54" s="6"/>
-      <c r="AL54" s="6"/>
-      <c r="AM54" s="6"/>
-      <c r="AN54" s="6"/>
-      <c r="AO54" s="6"/>
-    </row>
-    <row r="55" spans="26:41" x14ac:dyDescent="0.3">
-      <c r="AH55" s="6"/>
-      <c r="AI55" s="6"/>
-      <c r="AJ55" s="6"/>
-      <c r="AK55" s="6"/>
-      <c r="AL55" s="6"/>
-      <c r="AM55" s="6"/>
-      <c r="AN55" s="6"/>
-      <c r="AO55" s="6"/>
-    </row>
-    <row r="57" spans="26:41" x14ac:dyDescent="0.3">
+        <v>-38.747457995486876</v>
+      </c>
+    </row>
+    <row r="57" spans="26:32" x14ac:dyDescent="0.3">
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
     </row>

</xml_diff>